<commit_message>
Archivo para risk america
</commit_message>
<xml_diff>
--- a/Egresos.xlsx
+++ b/Egresos.xlsx
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>96586750-3/0</t>
+          <t>76529250-6/0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,29 +492,29 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1358</v>
+        <v>15</v>
       </c>
       <c r="E2" t="n">
-        <v>16958.5202</v>
+        <v>16956.9559</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17/03/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>17/03/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>23029670</v>
+        <v>254354</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>76529250-6/0</t>
+          <t>96586750-3/0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -528,23 +528,23 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>16958.5202</v>
+        <v>16956.9559</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17/03/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>17/03/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>1678893</v>
+        <v>135656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24-03 Checklist página principal
</commit_message>
<xml_diff>
--- a/Egresos.xlsx
+++ b/Egresos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CFINVSDPR</t>
+          <t>CFINHRFLA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -492,59 +492,23 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>9524</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>1319.635</v>
+        <v>16960.8644</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20/03/2025</t>
+          <t>21/03/2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>20/03/2025</t>
+          <t>21/03/2025</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>12568204</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>96921130-0/0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CFINHRFLA</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1157</v>
-      </c>
-      <c r="E3" t="n">
-        <v>16957.8775</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>20/03/2025</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20/03/2025</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>19620264</v>
+        <v>33922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>